<commit_message>
New calibration process to focus the paper. Still need to: 1. make a figure showing the parameter evolution (appendix?) 2. re-write the calibration section to better align with the new story. 3. consider deleting the existing appendix (calibration is nowhere near as good).
</commit_message>
<xml_diff>
--- a/input/sample_2/analytical calibration/calibration parameters.xlsx
+++ b/input/sample_2/analytical calibration/calibration parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pwal5\Documents\GitHub\SMAREACTcleaned\input\sample_2\analytical calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00158AD-0ED2-43B3-889D-BD0A14FD71D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0ADF8E-13E2-45E3-976E-11F4AB0A8921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{868CF7E1-07D3-4329-A985-3AC0D777E8EE}"/>
+    <workbookView xWindow="10260" yWindow="0" windowWidth="10260" windowHeight="13080" firstSheet="1" activeTab="1" xr2:uid="{868CF7E1-07D3-4329-A985-3AC0D777E8EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="2" r:id="rId1"/>
@@ -3021,10 +3021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6CA58A8-8AD1-46D1-9135-1155AFE94C1D}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3034,14 +3034,14 @@
     <col min="4" max="4" width="61.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -3082,8 +3082,9 @@
       <c r="D4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3098,7 +3099,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3113,7 +3114,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3128,7 +3129,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3143,7 +3144,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -3157,7 +3158,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -3171,7 +3172,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -3185,7 +3186,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -3199,7 +3200,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -3213,7 +3214,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -3227,7 +3228,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -3241,7 +3242,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -3561,8 +3562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82EE00C-5529-4307-9FE7-F3D1BFCE156B}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>